<commit_message>
avdia project data prepered
</commit_message>
<xml_diff>
--- a/yields_scraper/גמל_תשואות_מעובד.xlsx
+++ b/yields_scraper/גמל_תשואות_מעובד.xlsx
@@ -66,7 +66,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -80,6 +80,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -522,38 +525,38 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>0.84</v>
+        <v>0.96</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>81.3</v>
+        <v>82.40000000000001</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>958.46</v>
+        <v>1594.47</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3089.33</v>
+        <v>3808.88</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.57</v>
+        <v/>
       </c>
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>1.43</v>
+        <v>1.48</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>9.050000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>12.66</v>
+        <v>14.08</v>
       </c>
       <c r="J2" s="2" t="n">
-        <v>17.78</v>
+        <v>18.28</v>
       </c>
       <c r="K2" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L2" s="2" t="inlineStr">
@@ -570,35 +573,35 @@
         <v>-0.12</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>76.90000000000001</v>
+        <v>77.7</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>-14.77</v>
+        <v>17.17</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>1343.69</v>
+        <v>1401.69</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.58</v>
+        <v/>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.02</v>
       </c>
       <c r="G3" s="2" t="n">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>8.199999999999999</v>
+        <v>8.06</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>11.55</v>
+        <v>12.57</v>
       </c>
       <c r="J3" s="2" t="n">
-        <v>16.37</v>
+        <v>16.68</v>
       </c>
       <c r="K3" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L3" s="2" t="inlineStr">
@@ -612,218 +615,218 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>0.24</v>
+        <v>-0.48</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>79.2</v>
+        <v>77.09999999999999</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>212.22</v>
+        <v>-36.81</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>930.4</v>
+        <v>1559.66</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.63</v>
+        <v/>
       </c>
       <c r="F4" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>1.23</v>
+        <v>1.17</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>8.33</v>
+        <v>7.9</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>11.81</v>
+        <v>12.38</v>
       </c>
       <c r="J4" s="2" t="n">
-        <v>15.89</v>
+        <v>16.34</v>
       </c>
       <c r="K4" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L4" s="2" t="inlineStr">
         <is>
-          <t>מגדל גמל להשקעה כללי</t>
+          <t>כלל גמל לעתיד כללי</t>
         </is>
       </c>
       <c r="M4" s="2" t="n">
-        <v>7936</v>
+        <v>7988</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>-0.24</v>
+        <v>0.24</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>77</v>
+        <v>79.40000000000001</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>-72.11</v>
+        <v>261.67</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>1514.66</v>
+        <v>1010.07</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.66</v>
+        <v/>
       </c>
       <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G5" s="2" t="n">
-        <v>1.17</v>
+        <v>1.24</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>8.210000000000001</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>11.37</v>
+        <v>12.8</v>
       </c>
       <c r="J5" s="2" t="n">
-        <v>15.74</v>
+        <v>16.19</v>
       </c>
       <c r="K5" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>כלל גמל לעתיד כללי</t>
+          <t>מגדל גמל להשקעה כללי</t>
         </is>
       </c>
       <c r="M5" s="2" t="n">
-        <v>7988</v>
+        <v>7936</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>-0.36</v>
+        <v>0.6</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>80.90000000000001</v>
+        <v>82.3</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>481.07</v>
+        <v>668.98</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>2613.3</v>
+        <v>2936.52</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>0.62</v>
+        <v/>
       </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>1.17</v>
+        <v>1.24</v>
       </c>
       <c r="H6" s="2" t="n">
-        <v>8.279999999999999</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>11.7</v>
+        <v>13.13</v>
       </c>
       <c r="J6" s="2" t="n">
-        <v>15.25</v>
+        <v>15.44</v>
       </c>
       <c r="K6" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">הפניקס גמל להשקעה כללי </t>
+          <t xml:space="preserve">מיטב גמל להשקעה כללי </t>
         </is>
       </c>
       <c r="M6" s="2" t="n">
-        <v>7908</v>
+        <v>7978</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>0.72</v>
+        <v>-0.48</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>82</v>
+        <v>81.8</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>578.1799999999999</v>
+        <v>550.8200000000001</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>2717.33</v>
+        <v>2778.15</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.6</v>
+        <v/>
       </c>
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>1.23</v>
+        <v>1.17</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>8.460000000000001</v>
+        <v>8.06</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>11.96</v>
+        <v>12.82</v>
       </c>
       <c r="J7" s="2" t="n">
-        <v>14.96</v>
+        <v>15.24</v>
       </c>
       <c r="K7" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">מיטב גמל להשקעה כללי </t>
+          <t xml:space="preserve">הפניקס גמל להשקעה כללי </t>
         </is>
       </c>
       <c r="M7" s="2" t="n">
-        <v>7978</v>
+        <v>7908</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>0.96</v>
+        <v>0.72</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>80.8</v>
+        <v>81.3</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>718.79</v>
+        <v>787.9299999999999</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>5391.04</v>
+        <v>5530.75</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.74</v>
+        <v/>
       </c>
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G8" s="2" t="n">
-        <v>1.36</v>
+        <v>1.32</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>8.710000000000001</v>
+        <v>8.390000000000001</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>11.64</v>
+        <v>12.41</v>
       </c>
       <c r="J8" s="2" t="n">
-        <v>14.91</v>
+        <v>14.97</v>
       </c>
       <c r="K8" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L8" s="2" t="inlineStr">
@@ -840,35 +843,35 @@
         <v>0.96</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>91.5</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>977.02</v>
+        <v>954.86</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>3641.52</v>
+        <v>3814.34</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>0.63</v>
+        <v/>
       </c>
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="n">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>8.640000000000001</v>
+        <v>8.529999999999999</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>12.17</v>
+        <v>13.41</v>
       </c>
       <c r="J9" s="2" t="n">
-        <v>14.24</v>
+        <v>14.3</v>
       </c>
       <c r="K9" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L9" s="2" t="inlineStr">
@@ -885,35 +888,35 @@
         <v>0.96</v>
       </c>
       <c r="B10" s="3" t="n">
-        <v>90.09999999999999</v>
+        <v>90.2</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>340.6</v>
+        <v>144.66</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>3703.11</v>
+        <v>3723.45</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>0.6899999999999999</v>
+        <v/>
       </c>
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="n">
-        <v>1.16</v>
+        <v>1.14</v>
       </c>
       <c r="H10" s="2" t="n">
-        <v>8.48</v>
+        <v>8.31</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>12.11</v>
+        <v>13.11</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>13.07</v>
+        <v>13.52</v>
       </c>
       <c r="K10" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L10" s="2" t="inlineStr">
@@ -927,38 +930,38 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>-2.16</v>
+        <v>-2.4</v>
       </c>
       <c r="B11" s="3" t="n">
-        <v>85.7</v>
+        <v>86</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>-639.08</v>
+        <v>-803.5700000000001</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>4860.57</v>
+        <v>4829.77</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>0.65</v>
+        <v/>
       </c>
       <c r="F11" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G11" s="2" t="n">
-        <v>0.84</v>
+        <v>0.79</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>6.62</v>
+        <v>6.25</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>11.07</v>
+        <v>11.92</v>
       </c>
       <c r="J11" s="2" t="n">
-        <v>12.94</v>
+        <v>13.26</v>
       </c>
       <c r="K11" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L11" s="2" t="inlineStr">
@@ -974,21 +977,19 @@
       <c r="A12" s="5" t="inlineStr"/>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>83.8%</t>
+          <t>84.2%</t>
         </is>
       </c>
       <c r="C12" s="5" t="inlineStr">
         <is>
-          <t>3,540.4</t>
+          <t>4,140.2</t>
         </is>
       </c>
       <c r="D12" s="5" t="n">
-        <v>29804.95</v>
-      </c>
-      <c r="E12" s="5" t="inlineStr">
-        <is>
-          <t>0.65%</t>
-        </is>
+        <v>31393.28</v>
+      </c>
+      <c r="E12" s="5" t="n">
+        <v/>
       </c>
       <c r="F12" s="5" t="inlineStr">
         <is>
@@ -1002,22 +1003,22 @@
       </c>
       <c r="H12" s="5" t="inlineStr">
         <is>
-          <t>7.65%</t>
+          <t>7.44%</t>
         </is>
       </c>
       <c r="I12" s="5" t="inlineStr">
         <is>
-          <t>11.61%</t>
+          <t>12.65%</t>
         </is>
       </c>
       <c r="J12" s="5" t="inlineStr">
         <is>
-          <t>14.57%</t>
+          <t>14.96%</t>
         </is>
       </c>
       <c r="K12" s="6" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L12" s="5" t="inlineStr">
@@ -1096,38 +1097,38 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>1.2</v>
+        <v>0.96</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>90.2</v>
+        <v>89.90000000000001</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>1178.59</v>
+        <v>1641.49</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>2242.52</v>
+        <v>2811.74</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0.55</v>
+        <v/>
       </c>
       <c r="F16" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>1.52</v>
+        <v>1.56</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>15.94</v>
+        <v>15.67</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>22.58</v>
+        <v>25.71</v>
       </c>
       <c r="J16" s="2" t="n">
-        <v>32.78</v>
+        <v>33.35</v>
       </c>
       <c r="K16" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L16" s="2" t="inlineStr">
@@ -1141,128 +1142,130 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>-0.96</v>
+        <v>-3.72</v>
       </c>
       <c r="B17" s="3" t="n">
-        <v>93.09999999999999</v>
+        <v>90</v>
       </c>
       <c r="C17" s="3" t="n">
-        <v>255.79</v>
+        <v>107.88</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>622.55</v>
+        <v>672.65</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0.6</v>
+        <v/>
       </c>
       <c r="F17" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G17" s="2" t="n">
-        <v>1.23</v>
+        <v>1.07</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>13.59</v>
+        <v>11.75</v>
       </c>
       <c r="I17" s="2" t="n">
-        <v>18.89</v>
+        <v>19.3</v>
       </c>
       <c r="J17" s="2" t="n">
-        <v>25.95</v>
+        <v>27.3</v>
       </c>
       <c r="K17" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L17" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">מגדל גמל להשקעה מניות </t>
+          <t xml:space="preserve">כלל גמל לעתיד מניות </t>
         </is>
       </c>
       <c r="M17" s="2" t="n">
-        <v>7934</v>
+        <v>7991</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>-3.24</v>
+        <v>-1.08</v>
       </c>
       <c r="B18" s="3" t="n">
-        <v>90.09999999999999</v>
+        <v>92.7</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>79.78</v>
+        <v>312.06</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>629.55</v>
+        <v>705.62</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>0</v>
+        <v/>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - - -</t>
+        </is>
       </c>
       <c r="G18" s="2" t="n">
-        <v>1.07</v>
+        <v>1.24</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>12.46</v>
+        <v>13.27</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>16.82</v>
+        <v>21.14</v>
       </c>
       <c r="J18" s="2" t="n">
-        <v>25.83</v>
+        <v>26.73</v>
       </c>
       <c r="K18" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L18" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">כלל גמל לעתיד מניות </t>
+          <t xml:space="preserve">מגדל גמל להשקעה מניות </t>
         </is>
       </c>
       <c r="M18" s="2" t="n">
-        <v>7991</v>
+        <v>7934</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>0.24</v>
+        <v>-0.12</v>
       </c>
       <c r="B19" s="3" t="n">
-        <v>86.09999999999999</v>
+        <v>86.8</v>
       </c>
       <c r="C19" s="3" t="n">
-        <v>837.98</v>
+        <v>957.04</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>3955.46</v>
+        <v>4153.23</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0.74</v>
+        <v/>
       </c>
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G19" s="2" t="n">
-        <v>1.29</v>
+        <v>1.28</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>13.43</v>
+        <v>12.75</v>
       </c>
       <c r="I19" s="2" t="n">
-        <v>18.44</v>
+        <v>20.52</v>
       </c>
       <c r="J19" s="2" t="n">
-        <v>25.53</v>
+        <v>26.72</v>
       </c>
       <c r="K19" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L19" s="2" t="inlineStr">
@@ -1276,109 +1279,109 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>-1.92</v>
+        <v>-1.08</v>
       </c>
       <c r="B20" s="3" t="n">
-        <v>91.2</v>
+        <v>90.3</v>
       </c>
       <c r="C20" s="3" t="n">
-        <v>504.51</v>
+        <v>428.74</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>947.98</v>
+        <v>1242.38</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>0.64</v>
+        <v/>
       </c>
       <c r="F20" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>1.17</v>
+        <v>1.2</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>13</v>
+        <v>13.04</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>18.28</v>
+        <v>21.65</v>
       </c>
       <c r="J20" s="2" t="n">
-        <v>25.34</v>
+        <v>26.49</v>
       </c>
       <c r="K20" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L20" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">הפניקס גמל להשקעה מניות </t>
+          <t xml:space="preserve">מיטב גמל להשקעה מניות </t>
         </is>
       </c>
       <c r="M20" s="2" t="n">
-        <v>7975</v>
+        <v>7860</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>-0.72</v>
+        <v>-2.16</v>
       </c>
       <c r="B21" s="3" t="n">
-        <v>90.09999999999999</v>
+        <v>91.59999999999999</v>
       </c>
       <c r="C21" s="3" t="n">
-        <v>336.52</v>
+        <v>622.35</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>1106.47</v>
+        <v>1105.58</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>0.58</v>
+        <v/>
       </c>
       <c r="F21" s="2" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G21" s="2" t="n">
-        <v>1.19</v>
+        <v>1.18</v>
       </c>
       <c r="H21" s="2" t="n">
-        <v>13.56</v>
+        <v>12.61</v>
       </c>
       <c r="I21" s="2" t="n">
-        <v>19.02</v>
+        <v>20.85</v>
       </c>
       <c r="J21" s="2" t="n">
-        <v>25.22</v>
+        <v>25.89</v>
       </c>
       <c r="K21" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L21" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">מיטב גמל להשקעה מניות </t>
+          <t xml:space="preserve">הפניקס גמל להשקעה מניות </t>
         </is>
       </c>
       <c r="M21" s="2" t="n">
-        <v>7860</v>
+        <v>7975</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>1.2</v>
+        <v>1.08</v>
       </c>
       <c r="B22" s="3" t="n">
-        <v>93.2</v>
+        <v>93.3</v>
       </c>
       <c r="C22" s="3" t="n">
-        <v>424.8</v>
+        <v>283.7</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>3356.86</v>
+        <v>3409.87</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>0.68</v>
+        <v/>
       </c>
       <c r="F22" s="2" t="n">
         <v>0</v>
@@ -1387,17 +1390,17 @@
         <v>1.25</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>14.45</v>
+        <v>14</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>19.42</v>
+        <v>21.64</v>
       </c>
       <c r="J22" s="2" t="n">
-        <v>20.67</v>
+        <v>22.01</v>
       </c>
       <c r="K22" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L22" s="2" t="inlineStr">
@@ -1411,38 +1414,38 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>-4.44</v>
+        <v>-4.92</v>
       </c>
       <c r="B23" s="3" t="n">
-        <v>89.59999999999999</v>
+        <v>90.2</v>
       </c>
       <c r="C23" s="3" t="n">
-        <v>-193.84</v>
+        <v>-244.03</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>4551.23</v>
+        <v>4530.61</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>0.61</v>
+        <v/>
       </c>
       <c r="F23" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G23" s="2" t="n">
-        <v>0.91</v>
+        <v>0.86</v>
       </c>
       <c r="H23" s="2" t="n">
-        <v>10.44</v>
+        <v>9.720000000000001</v>
       </c>
       <c r="I23" s="2" t="n">
-        <v>17.72</v>
+        <v>19.42</v>
       </c>
       <c r="J23" s="2" t="n">
-        <v>20.08</v>
+        <v>20.86</v>
       </c>
       <c r="K23" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L23" s="2" t="inlineStr">
@@ -1456,38 +1459,38 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>0.36</v>
+        <v>0.12</v>
       </c>
       <c r="B24" s="3" t="n">
-        <v>95.09999999999999</v>
+        <v>95.3</v>
       </c>
       <c r="C24" s="3" t="n">
-        <v>1293.19</v>
+        <v>1152.22</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>5776.41</v>
+        <v>5946.47</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0.63</v>
+        <v/>
       </c>
       <c r="F24" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>1.13</v>
+        <v>1.11</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>13.88</v>
+        <v>13.39</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>19.69</v>
+        <v>22.24</v>
       </c>
       <c r="J24" s="2" t="n">
-        <v>20.04</v>
+        <v>20.7</v>
       </c>
       <c r="K24" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L24" s="2" t="inlineStr">
@@ -1505,13 +1508,13 @@
         <v>98.90000000000001</v>
       </c>
       <c r="C25" s="3" t="n">
-        <v>14.24</v>
+        <v>14.97</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>225.74</v>
+        <v>228.36</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.59</v>
+        <v/>
       </c>
       <c r="F25" s="2" t="n">
         <v>0.01</v>
@@ -1527,14 +1530,14 @@
         </is>
       </c>
       <c r="I25" s="2" t="n">
-        <v>16.03</v>
+        <v>16.04</v>
       </c>
       <c r="J25" s="2" t="n">
-        <v>11.42</v>
+        <v>9.789999999999999</v>
       </c>
       <c r="K25" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L25" s="2" t="inlineStr">
@@ -1550,21 +1553,19 @@
       <c r="A26" s="5" t="inlineStr"/>
       <c r="B26" s="5" t="inlineStr">
         <is>
-          <t>91.2%</t>
+          <t>91.5%</t>
         </is>
       </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
-          <t>4,731.6</t>
+          <t>5,276.4</t>
         </is>
       </c>
       <c r="D26" s="5" t="n">
-        <v>23414.77</v>
-      </c>
-      <c r="E26" s="5" t="inlineStr">
-        <is>
-          <t>0.64%</t>
-        </is>
+        <v>24806.51</v>
+      </c>
+      <c r="E26" s="5" t="n">
+        <v/>
       </c>
       <c r="F26" s="5" t="inlineStr">
         <is>
@@ -1578,22 +1579,22 @@
       </c>
       <c r="H26" s="5" t="inlineStr">
         <is>
-          <t>12.05%</t>
+          <t>11.56%</t>
         </is>
       </c>
       <c r="I26" s="5" t="inlineStr">
         <is>
-          <t>18.61%</t>
+          <t>20.86%</t>
         </is>
       </c>
       <c r="J26" s="5" t="inlineStr">
         <is>
-          <t>22.23%</t>
+          <t>23.42%</t>
         </is>
       </c>
       <c r="K26" s="6" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L26" s="5" t="inlineStr">
@@ -1672,38 +1673,38 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>3.48</v>
+        <v>3.36</v>
       </c>
       <c r="B30" s="3" t="n">
-        <v>97.90000000000001</v>
+        <v>98.3</v>
       </c>
       <c r="C30" s="3" t="n">
-        <v>8.76</v>
+        <v>-75.72</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>1424.63</v>
+        <v>1370.34</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0.55</v>
+        <v/>
       </c>
       <c r="F30" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G30" s="2" t="n">
-        <v>1.13</v>
+        <v>1.01</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>14.53</v>
+        <v>13.94</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>19.24</v>
+        <v>18.9</v>
       </c>
       <c r="J30" s="2" t="n">
-        <v>3.41</v>
+        <v>3.05</v>
       </c>
       <c r="K30" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L30" s="2" t="inlineStr">
@@ -1716,113 +1717,111 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="inlineStr"/>
+      <c r="A31" s="2" t="n">
+        <v>3.6</v>
+      </c>
       <c r="B31" s="3" t="n">
-        <v>96.3</v>
+        <v>99.2</v>
       </c>
       <c r="C31" s="3" t="n">
-        <v>63.74</v>
+        <v>9.49</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>737.8200000000001</v>
+        <v>3822.52</v>
       </c>
       <c r="E31" s="2" t="n">
-        <v>0.51</v>
+        <v/>
       </c>
       <c r="F31" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G31" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - - -</t>
-        </is>
-      </c>
-      <c r="H31" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - - -</t>
-        </is>
+      <c r="G31" s="2" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>14.02</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>18.81</v>
+        <v>18.73</v>
       </c>
       <c r="J31" s="2" t="n">
-        <v>3.17</v>
+        <v>2.94</v>
       </c>
       <c r="K31" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L31" s="2" t="inlineStr">
         <is>
-          <t>מנורה מבטחים גמל להשקעה עוקב S&amp;P500</t>
+          <t>הפניקס גמל להשקעה עוקב מדד S&amp;P500</t>
         </is>
       </c>
       <c r="M31" s="2" t="n">
-        <v>13874</v>
+        <v>13250</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>3.72</v>
+        <v>2.88</v>
       </c>
       <c r="B32" s="3" t="n">
-        <v>99.3</v>
+        <v>98</v>
       </c>
       <c r="C32" s="3" t="n">
-        <v>277.26</v>
+        <v>-251.08</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>3975.69</v>
+        <v>1489.5</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>0.57</v>
+        <v/>
       </c>
       <c r="F32" s="2" t="n">
         <v>0</v>
       </c>
       <c r="G32" s="2" t="n">
-        <v>1.15</v>
+        <v>0.96</v>
       </c>
       <c r="H32" s="2" t="n">
-        <v>14.67</v>
+        <v>13.21</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>18.48</v>
+        <v>18.23</v>
       </c>
       <c r="J32" s="2" t="n">
-        <v>3.16</v>
+        <v>2.91</v>
       </c>
       <c r="K32" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L32" s="2" t="inlineStr">
         <is>
-          <t>הפניקס גמל להשקעה עוקב מדד S&amp;P500</t>
+          <t>מור גמל להשקעה - עוקב מדד S&amp;P500</t>
         </is>
       </c>
       <c r="M32" s="2" t="n">
-        <v>13250</v>
+        <v>7958</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr"/>
       <c r="B33" s="3" t="n">
-        <v>98.90000000000001</v>
+        <v>95.8</v>
       </c>
       <c r="C33" s="3" t="n">
-        <v>285.31</v>
+        <v>14.19</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>931.9400000000001</v>
+        <v>715.7</v>
       </c>
       <c r="E33" s="2" t="n">
-        <v>0.57</v>
+        <v/>
       </c>
       <c r="F33" s="2" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="G33" s="2" t="inlineStr">
         <is>
@@ -1835,38 +1834,38 @@
         </is>
       </c>
       <c r="I33" s="2" t="n">
-        <v>19.03</v>
+        <v>18.33</v>
       </c>
       <c r="J33" s="2" t="n">
-        <v>3.06</v>
+        <v>2.9</v>
       </c>
       <c r="K33" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L33" s="2" t="inlineStr">
         <is>
-          <t>מגדל גמל להשקעה עוקב מדד s&amp;p500</t>
+          <t>מנורה מבטחים גמל להשקעה עוקב S&amp;P500</t>
         </is>
       </c>
       <c r="M33" s="2" t="n">
-        <v>13563</v>
+        <v>13874</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr"/>
       <c r="B34" s="3" t="n">
-        <v>99.3</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="C34" s="3" t="n">
-        <v>209.86</v>
+        <v>98.01000000000001</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>1005.58</v>
+        <v>970.85</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>0.54</v>
+        <v/>
       </c>
       <c r="F34" s="2" t="n">
         <v>0</v>
@@ -1887,11 +1886,11 @@
         </is>
       </c>
       <c r="J34" s="2" t="n">
-        <v>2.91</v>
+        <v>2.88</v>
       </c>
       <c r="K34" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L34" s="2" t="inlineStr">
@@ -1906,108 +1905,112 @@
     <row r="35">
       <c r="A35" s="2" t="inlineStr"/>
       <c r="B35" s="3" t="n">
+        <v>99.40000000000001</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>230.1</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>921.16</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v/>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - - -</t>
+        </is>
+      </c>
+      <c r="G35" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - - -</t>
+        </is>
+      </c>
+      <c r="H35" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> - - -</t>
+        </is>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>18.65</v>
+      </c>
+      <c r="J35" s="2" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="K35" s="4" t="inlineStr">
+        <is>
+          <t>12/25-01/25</t>
+        </is>
+      </c>
+      <c r="L35" s="2" t="inlineStr">
+        <is>
+          <t>מגדל גמל להשקעה עוקב מדד s&amp;p500</t>
+        </is>
+      </c>
+      <c r="M35" s="2" t="n">
+        <v>13563</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr"/>
+      <c r="B36" s="3" t="n">
         <v>98.59999999999999</v>
       </c>
-      <c r="C35" s="3" t="n">
-        <v>356.17</v>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>2214.98</v>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="F35" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" s="2" t="inlineStr">
+      <c r="C36" s="3" t="n">
+        <v>228.59</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>2174.63</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v/>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> - - -</t>
         </is>
       </c>
-      <c r="H35" s="2" t="inlineStr">
+      <c r="H36" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> - - -</t>
         </is>
       </c>
-      <c r="I35" s="2" t="n">
-        <v>19.22</v>
-      </c>
-      <c r="J35" s="2" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="K35" s="4" t="inlineStr">
-        <is>
-          <t>11/25-12/24</t>
-        </is>
-      </c>
-      <c r="L35" s="2" t="inlineStr">
+      <c r="I36" s="2" t="n">
+        <v>18.81</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="K36" s="4" t="inlineStr">
+        <is>
+          <t>12/25-01/25</t>
+        </is>
+      </c>
+      <c r="L36" s="2" t="inlineStr">
         <is>
           <t>הראל גמל להשקעה עוקב מדד s&amp;p 500</t>
         </is>
       </c>
-      <c r="M35" s="2" t="n">
+      <c r="M36" s="2" t="n">
         <v>13414</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B36" s="3" t="n">
-        <v>98.3</v>
-      </c>
-      <c r="C36" s="3" t="n">
-        <v>-134.49</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <v>1573.72</v>
-      </c>
-      <c r="E36" s="2" t="n">
-        <v>0.72</v>
-      </c>
-      <c r="F36" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" s="2" t="n">
-        <v>1.06</v>
-      </c>
-      <c r="H36" s="2" t="n">
-        <v>13.72</v>
-      </c>
-      <c r="I36" s="2" t="n">
-        <v>17.84</v>
-      </c>
-      <c r="J36" s="2" t="n">
-        <v>2.83</v>
-      </c>
-      <c r="K36" s="4" t="inlineStr">
-        <is>
-          <t>11/25-12/24</t>
-        </is>
-      </c>
-      <c r="L36" s="2" t="inlineStr">
-        <is>
-          <t>מור גמל להשקעה - עוקב מדד S&amp;P500</t>
-        </is>
-      </c>
-      <c r="M36" s="2" t="n">
-        <v>7958</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr"/>
       <c r="B37" s="3" t="n">
-        <v>98.7</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="C37" s="3" t="n">
-        <v>46.24</v>
+        <v>-93.45999999999999</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>944.03</v>
+        <v>1218.4</v>
       </c>
       <c r="E37" s="2" t="n">
-        <v>0.61</v>
+        <v/>
       </c>
       <c r="F37" s="2" t="n">
         <v>0</v>
@@ -2023,114 +2026,108 @@
         </is>
       </c>
       <c r="I37" s="2" t="n">
-        <v>18.4</v>
+        <v>18.21</v>
       </c>
       <c r="J37" s="2" t="n">
-        <v>2.78</v>
+        <v>2.58</v>
       </c>
       <c r="K37" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L37" s="2" t="inlineStr">
         <is>
-          <t>כלל גמל לעתיד עוקב  מדד s&amp;p 500</t>
+          <t>אנליסט קופת גמל להשקעה עוקב מדד S&amp;P500</t>
         </is>
       </c>
       <c r="M37" s="2" t="n">
-        <v>13344</v>
+        <v>13854</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="inlineStr"/>
+      <c r="A38" s="2" t="n">
+        <v>3.24</v>
+      </c>
       <c r="B38" s="3" t="n">
         <v>98.59999999999999</v>
       </c>
       <c r="C38" s="3" t="n">
-        <v>31.41</v>
+        <v>-13.26</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>1282.7</v>
+        <v>907.37</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>0.58</v>
+        <v/>
       </c>
       <c r="F38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G38" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - - -</t>
-        </is>
-      </c>
-      <c r="H38" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - - -</t>
-        </is>
+      <c r="G38" s="2" t="n">
+        <v>1.01</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>13.87</v>
       </c>
       <c r="I38" s="2" t="n">
-        <v>18.09</v>
+        <v>18.33</v>
       </c>
       <c r="J38" s="2" t="n">
-        <v>2.73</v>
+        <v>2.5</v>
       </c>
       <c r="K38" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L38" s="2" t="inlineStr">
         <is>
-          <t>אנליסט קופת גמל להשקעה עוקב מדד S&amp;P500</t>
+          <t>כלל גמל לעתיד עוקב  מדד s&amp;p 500</t>
         </is>
       </c>
       <c r="M38" s="2" t="n">
-        <v>13854</v>
+        <v>13344</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="inlineStr"/>
       <c r="B39" s="3" t="n">
-        <v>99.2</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="C39" s="3" t="n">
-        <v>83.06999999999999</v>
+        <v>44.63</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>137.01</v>
-      </c>
-      <c r="E39" s="2" t="inlineStr">
+        <v>131.62</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v/>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> - - -</t>
         </is>
       </c>
-      <c r="F39" s="2" t="inlineStr">
+      <c r="H39" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> - - -</t>
         </is>
       </c>
-      <c r="G39" s="2" t="inlineStr">
+      <c r="I39" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> - - -</t>
         </is>
       </c>
-      <c r="H39" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - - -</t>
-        </is>
-      </c>
-      <c r="I39" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> - - -</t>
-        </is>
-      </c>
       <c r="J39" s="2" t="n">
-        <v>2.6</v>
+        <v>2.39</v>
       </c>
       <c r="K39" s="4" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L39" s="2" t="inlineStr">
@@ -2149,18 +2146,14 @@
           <t>98.7%</t>
         </is>
       </c>
-      <c r="C40" s="5" t="inlineStr">
-        <is>
-          <t>1,227.3</t>
-        </is>
+      <c r="C40" s="7" t="n">
+        <v>191.5</v>
       </c>
       <c r="D40" s="5" t="n">
-        <v>14228.1</v>
-      </c>
-      <c r="E40" s="5" t="inlineStr">
-        <is>
-          <t>0.58%</t>
-        </is>
+        <v>13722.09</v>
+      </c>
+      <c r="E40" s="5" t="n">
+        <v/>
       </c>
       <c r="F40" s="5" t="inlineStr">
         <is>
@@ -2174,22 +2167,22 @@
       </c>
       <c r="H40" s="5" t="inlineStr">
         <is>
-          <t>14.47%</t>
+          <t>13.90%</t>
         </is>
       </c>
       <c r="I40" s="5" t="inlineStr">
         <is>
-          <t>18.56%</t>
+          <t>18.64%</t>
         </is>
       </c>
       <c r="J40" s="5" t="inlineStr">
         <is>
-          <t>3.02%</t>
+          <t>2.83%</t>
         </is>
       </c>
       <c r="K40" s="6" t="inlineStr">
         <is>
-          <t>11/25-12/24</t>
+          <t>12/25-01/25</t>
         </is>
       </c>
       <c r="L40" s="5" t="inlineStr">

</xml_diff>